<commit_message>
SLICE-FOS Salary Download Link still pending
</commit_message>
<xml_diff>
--- a/media/SLICE/Billing/FEB 22/SLICE BILLING.xlsx
+++ b/media/SLICE/Billing/FEB 22/SLICE BILLING.xlsx
@@ -532,7 +532,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -700,7 +700,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -754,7 +754,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -808,7 +808,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -862,7 +862,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -916,7 +916,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -970,7 +970,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1510,7 +1510,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1624,7 +1624,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1678,7 +1678,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1786,7 +1786,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1900,7 +1900,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -2182,7 +2182,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2236,7 +2236,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -2290,7 +2290,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SURESH</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2398,7 +2398,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2560,7 +2560,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2614,7 +2614,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2788,7 +2788,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2844,7 +2844,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2898,7 +2898,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2952,7 +2952,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -3012,7 +3012,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -3066,7 +3066,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -3120,7 +3120,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -3174,7 +3174,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -3228,7 +3228,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -3282,7 +3282,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
@@ -3336,7 +3336,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -3396,7 +3396,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -3450,7 +3450,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -3510,7 +3510,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -3570,7 +3570,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -3624,7 +3624,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -3678,7 +3678,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -3732,7 +3732,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -3786,7 +3786,7 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>RAJENDER KUMAR VERMA</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
@@ -3840,7 +3840,7 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>GIRJESH KUMAR</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
@@ -3894,7 +3894,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -3948,7 +3948,7 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
@@ -4002,7 +4002,7 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
@@ -4056,7 +4056,7 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
@@ -4116,7 +4116,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -4170,7 +4170,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -4224,7 +4224,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -4278,7 +4278,7 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
@@ -4332,7 +4332,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
@@ -4386,7 +4386,7 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
@@ -4440,7 +4440,7 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
@@ -4500,7 +4500,7 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
@@ -4554,7 +4554,7 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
@@ -4614,7 +4614,7 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
@@ -4668,7 +4668,7 @@
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
@@ -4728,7 +4728,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -4782,7 +4782,7 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
@@ -4836,7 +4836,7 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
@@ -4890,7 +4890,7 @@
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
@@ -4944,7 +4944,7 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
@@ -4998,7 +4998,7 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
@@ -5052,7 +5052,7 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
@@ -5106,7 +5106,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -5166,7 +5166,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -5226,7 +5226,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -5280,7 +5280,7 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
@@ -5334,7 +5334,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -5394,7 +5394,7 @@
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
@@ -5448,7 +5448,7 @@
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
@@ -5508,7 +5508,7 @@
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
@@ -5562,7 +5562,7 @@
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
@@ -5616,7 +5616,7 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
@@ -5670,7 +5670,7 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
@@ -5724,7 +5724,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -5778,7 +5778,7 @@
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H97" t="inlineStr">
@@ -5834,7 +5834,7 @@
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
@@ -5888,7 +5888,7 @@
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
@@ -5942,7 +5942,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
@@ -6002,7 +6002,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
@@ -6062,7 +6062,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H102" t="inlineStr">
@@ -6116,7 +6116,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SURESH</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
@@ -6170,7 +6170,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
@@ -6230,7 +6230,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
@@ -6284,7 +6284,7 @@
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H106" t="inlineStr">
@@ -6338,7 +6338,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
@@ -6392,7 +6392,7 @@
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H108" t="inlineStr">
@@ -6452,7 +6452,7 @@
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H109" t="inlineStr">
@@ -6512,7 +6512,7 @@
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H110" t="inlineStr">
@@ -6572,7 +6572,7 @@
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H111" t="inlineStr">
@@ -6632,7 +6632,7 @@
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H112" t="inlineStr">
@@ -6692,7 +6692,7 @@
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H113" t="inlineStr">
@@ -6752,7 +6752,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
@@ -6806,7 +6806,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
@@ -6866,7 +6866,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
@@ -6920,7 +6920,7 @@
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H117" t="inlineStr">
@@ -6974,7 +6974,7 @@
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H118" t="inlineStr">
@@ -7028,7 +7028,7 @@
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H119" t="inlineStr">
@@ -7082,7 +7082,7 @@
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H120" t="inlineStr">
@@ -7136,7 +7136,7 @@
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H121" t="inlineStr">
@@ -7190,7 +7190,7 @@
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H122" t="inlineStr">
@@ -7250,7 +7250,7 @@
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H123" t="inlineStr">
@@ -7304,7 +7304,7 @@
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H124" t="inlineStr">
@@ -7358,7 +7358,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
@@ -7412,7 +7412,7 @@
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
@@ -7466,7 +7466,7 @@
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H127" t="inlineStr">
@@ -7520,7 +7520,7 @@
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
@@ -7580,7 +7580,7 @@
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H129" t="inlineStr">
@@ -7640,7 +7640,7 @@
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
@@ -7694,7 +7694,7 @@
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H131" t="inlineStr">
@@ -7748,7 +7748,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -7808,7 +7808,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
@@ -7862,7 +7862,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
@@ -7916,7 +7916,7 @@
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H135" t="inlineStr">
@@ -7970,7 +7970,7 @@
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
@@ -8024,7 +8024,7 @@
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H137" t="inlineStr">
@@ -8078,7 +8078,7 @@
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
@@ -8132,7 +8132,7 @@
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
@@ -8186,7 +8186,7 @@
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H140" t="inlineStr">
@@ -8240,7 +8240,7 @@
       </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
@@ -8294,7 +8294,7 @@
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H142" t="inlineStr">
@@ -8348,7 +8348,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
@@ -8402,7 +8402,7 @@
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H144" t="inlineStr">
@@ -8456,7 +8456,7 @@
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
@@ -8510,7 +8510,7 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
@@ -8564,7 +8564,7 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
@@ -8618,7 +8618,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H148" t="inlineStr">
@@ -8672,7 +8672,7 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H149" t="inlineStr">
@@ -8726,7 +8726,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
@@ -8780,7 +8780,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
@@ -8834,7 +8834,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H152" t="inlineStr">
@@ -8888,7 +8888,7 @@
       </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H153" t="inlineStr">
@@ -8942,7 +8942,7 @@
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H154" t="inlineStr">
@@ -8996,7 +8996,7 @@
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H155" t="inlineStr">
@@ -9050,7 +9050,7 @@
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
@@ -9104,7 +9104,7 @@
       </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ARVIND KUMAR</t>
         </is>
       </c>
       <c r="H157" t="inlineStr">
@@ -9164,7 +9164,7 @@
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
@@ -9218,7 +9218,7 @@
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H159" t="inlineStr">
@@ -9278,7 +9278,7 @@
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H160" t="inlineStr">
@@ -9332,7 +9332,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
@@ -9386,7 +9386,7 @@
       </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H162" t="inlineStr">
@@ -9440,7 +9440,7 @@
       </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H163" t="inlineStr">
@@ -9494,7 +9494,7 @@
       </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H164" t="inlineStr">
@@ -9548,7 +9548,7 @@
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>GURPREET SINGH</t>
         </is>
       </c>
       <c r="H165" t="inlineStr">
@@ -9602,7 +9602,7 @@
       </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H166" t="inlineStr">
@@ -9662,7 +9662,7 @@
       </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H167" t="inlineStr">
@@ -9718,7 +9718,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
@@ -9772,7 +9772,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H169" t="inlineStr">
@@ -9826,7 +9826,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H170" t="inlineStr">
@@ -9886,7 +9886,7 @@
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H171" t="inlineStr">
@@ -9940,7 +9940,7 @@
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H172" t="inlineStr">
@@ -10000,7 +10000,7 @@
       </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H173" t="inlineStr">
@@ -10054,7 +10054,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H174" t="inlineStr">
@@ -10108,7 +10108,7 @@
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H175" t="inlineStr">
@@ -10162,7 +10162,7 @@
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
@@ -10216,7 +10216,7 @@
       </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H177" t="inlineStr">
@@ -10270,7 +10270,7 @@
       </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>RAJENDER KUMAR VERMA</t>
         </is>
       </c>
       <c r="H178" t="inlineStr">
@@ -10330,7 +10330,7 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H179" t="inlineStr">
@@ -10384,7 +10384,7 @@
       </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H180" t="inlineStr">
@@ -10444,7 +10444,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
@@ -10498,7 +10498,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H182" t="inlineStr">
@@ -10552,7 +10552,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H183" t="inlineStr">
@@ -10606,7 +10606,7 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H184" t="inlineStr">
@@ -10660,7 +10660,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
@@ -10714,7 +10714,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
@@ -10768,7 +10768,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
@@ -10822,7 +10822,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
@@ -10876,7 +10876,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H189" t="inlineStr">
@@ -10936,7 +10936,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
@@ -10996,7 +10996,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
@@ -11056,7 +11056,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H192" t="inlineStr">
@@ -11110,7 +11110,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
@@ -11170,7 +11170,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H194" t="inlineStr">
@@ -11224,7 +11224,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
@@ -11278,7 +11278,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
@@ -11338,7 +11338,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ARVIND KUMAR</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
@@ -11392,7 +11392,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H198" t="inlineStr">
@@ -11446,7 +11446,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
@@ -11500,7 +11500,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
@@ -11554,7 +11554,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
@@ -11614,7 +11614,7 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H202" t="inlineStr">
@@ -11668,7 +11668,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H203" t="inlineStr">
@@ -11722,7 +11722,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
@@ -11782,7 +11782,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H205" t="inlineStr">
@@ -11836,7 +11836,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
@@ -11890,7 +11890,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H207" t="inlineStr">
@@ -11944,7 +11944,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
@@ -11998,7 +11998,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
@@ -12052,7 +12052,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
@@ -12112,7 +12112,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
@@ -12166,7 +12166,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H212" t="inlineStr">
@@ -12226,7 +12226,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
@@ -12280,7 +12280,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
@@ -12334,7 +12334,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H215" t="inlineStr">
@@ -12394,7 +12394,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
@@ -12450,7 +12450,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
@@ -12504,7 +12504,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H218" t="inlineStr">
@@ -12564,7 +12564,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
@@ -12618,7 +12618,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
@@ -12678,7 +12678,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
@@ -12732,7 +12732,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
@@ -12786,7 +12786,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
@@ -12846,7 +12846,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SURESH</t>
         </is>
       </c>
       <c r="H224" t="inlineStr">
@@ -12900,7 +12900,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
@@ -12960,7 +12960,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
@@ -13014,7 +13014,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
@@ -13068,7 +13068,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
@@ -13122,7 +13122,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H229" t="inlineStr">
@@ -13182,7 +13182,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H230" t="inlineStr">
@@ -13242,7 +13242,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
@@ -13296,7 +13296,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>GURPREET SINGH</t>
         </is>
       </c>
       <c r="H232" t="inlineStr">
@@ -13350,7 +13350,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
@@ -13404,7 +13404,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
@@ -13464,7 +13464,7 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SURESH</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
@@ -13518,7 +13518,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
@@ -13572,7 +13572,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H237" t="inlineStr">
@@ -13626,7 +13626,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
@@ -13680,7 +13680,7 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H239" t="inlineStr">
@@ -13734,7 +13734,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H240" t="inlineStr">
@@ -13788,7 +13788,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H241" t="inlineStr">
@@ -13842,7 +13842,7 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H242" t="inlineStr">
@@ -13896,7 +13896,7 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H243" t="inlineStr">
@@ -13950,7 +13950,7 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">
@@ -14004,7 +14004,7 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H245" t="inlineStr">
@@ -14064,7 +14064,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
@@ -14118,7 +14118,7 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H247" t="inlineStr">
@@ -14178,7 +14178,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H248" t="inlineStr">
@@ -14238,7 +14238,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
@@ -14292,7 +14292,7 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H250" t="inlineStr">
@@ -14346,7 +14346,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
@@ -14400,7 +14400,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H252" t="inlineStr">
@@ -14454,7 +14454,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H253" t="inlineStr">
@@ -14508,7 +14508,7 @@
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H254" t="inlineStr">
@@ -14568,7 +14568,7 @@
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H255" t="inlineStr">
@@ -14622,7 +14622,7 @@
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H256" t="inlineStr">
@@ -14676,7 +14676,7 @@
       </c>
       <c r="G257" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H257" t="inlineStr">
@@ -14730,7 +14730,7 @@
       </c>
       <c r="G258" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H258" t="inlineStr">
@@ -14784,7 +14784,7 @@
       </c>
       <c r="G259" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUKHVINDER SINGH</t>
         </is>
       </c>
       <c r="H259" t="inlineStr">
@@ -14838,7 +14838,7 @@
       </c>
       <c r="G260" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ARVIND KUMAR</t>
         </is>
       </c>
       <c r="H260" t="inlineStr">
@@ -14892,7 +14892,7 @@
       </c>
       <c r="G261" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H261" t="inlineStr">
@@ -14952,7 +14952,7 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H262" t="inlineStr">
@@ -15012,7 +15012,7 @@
       </c>
       <c r="G263" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H263" t="inlineStr">
@@ -15072,7 +15072,7 @@
       </c>
       <c r="G264" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H264" t="inlineStr">
@@ -15126,7 +15126,7 @@
       </c>
       <c r="G265" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H265" t="inlineStr">
@@ -15186,7 +15186,7 @@
       </c>
       <c r="G266" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H266" t="inlineStr">
@@ -15246,7 +15246,7 @@
       </c>
       <c r="G267" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H267" t="inlineStr">
@@ -15300,7 +15300,7 @@
       </c>
       <c r="G268" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H268" t="inlineStr">
@@ -15360,7 +15360,7 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H269" t="inlineStr">
@@ -15420,7 +15420,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H270" t="inlineStr">
@@ -15480,7 +15480,7 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H271" t="inlineStr">
@@ -15540,7 +15540,7 @@
       </c>
       <c r="G272" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>GURPREET SINGH</t>
         </is>
       </c>
       <c r="H272" t="inlineStr">
@@ -15594,7 +15594,7 @@
       </c>
       <c r="G273" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H273" t="inlineStr">
@@ -15648,7 +15648,7 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H274" t="inlineStr">
@@ -15702,7 +15702,7 @@
       </c>
       <c r="G275" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H275" t="inlineStr">
@@ -15756,7 +15756,7 @@
       </c>
       <c r="G276" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H276" t="inlineStr">
@@ -15810,7 +15810,7 @@
       </c>
       <c r="G277" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H277" t="inlineStr">
@@ -15870,7 +15870,7 @@
       </c>
       <c r="G278" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H278" t="inlineStr">
@@ -15924,7 +15924,7 @@
       </c>
       <c r="G279" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H279" t="inlineStr">
@@ -15978,7 +15978,7 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H280" t="inlineStr">
@@ -16032,7 +16032,7 @@
       </c>
       <c r="G281" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H281" t="inlineStr">
@@ -16086,7 +16086,7 @@
       </c>
       <c r="G282" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H282" t="inlineStr">
@@ -16140,7 +16140,7 @@
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H283" t="inlineStr">
@@ -16200,7 +16200,7 @@
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H284" t="inlineStr">
@@ -16260,7 +16260,7 @@
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H285" t="inlineStr">
@@ -16314,7 +16314,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H286" t="inlineStr">
@@ -16368,7 +16368,7 @@
       </c>
       <c r="G287" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>MANOJ TOMAR</t>
         </is>
       </c>
       <c r="H287" t="inlineStr">
@@ -16422,7 +16422,7 @@
       </c>
       <c r="G288" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H288" t="inlineStr">
@@ -16482,7 +16482,7 @@
       </c>
       <c r="G289" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H289" t="inlineStr">
@@ -16542,7 +16542,7 @@
       </c>
       <c r="G290" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H290" t="inlineStr">
@@ -16596,7 +16596,7 @@
       </c>
       <c r="G291" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H291" t="inlineStr">
@@ -16656,7 +16656,7 @@
       </c>
       <c r="G292" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H292" t="inlineStr">
@@ -16716,7 +16716,7 @@
       </c>
       <c r="G293" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H293" t="inlineStr">
@@ -16776,7 +16776,7 @@
       </c>
       <c r="G294" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H294" t="inlineStr">
@@ -16836,7 +16836,7 @@
       </c>
       <c r="G295" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H295" t="inlineStr">
@@ -16890,7 +16890,7 @@
       </c>
       <c r="G296" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H296" t="inlineStr">
@@ -16944,7 +16944,7 @@
       </c>
       <c r="G297" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H297" t="inlineStr">
@@ -16998,7 +16998,7 @@
       </c>
       <c r="G298" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H298" t="inlineStr">
@@ -17052,7 +17052,7 @@
       </c>
       <c r="G299" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H299" t="inlineStr">
@@ -17106,7 +17106,7 @@
       </c>
       <c r="G300" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H300" t="inlineStr">
@@ -17160,7 +17160,7 @@
       </c>
       <c r="G301" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H301" t="inlineStr">
@@ -17220,7 +17220,7 @@
       </c>
       <c r="G302" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H302" t="inlineStr">
@@ -17274,7 +17274,7 @@
       </c>
       <c r="G303" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H303" t="inlineStr">
@@ -17328,7 +17328,7 @@
       </c>
       <c r="G304" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>GIRJESH KUMAR</t>
         </is>
       </c>
       <c r="H304" t="inlineStr">
@@ -17388,7 +17388,7 @@
       </c>
       <c r="G305" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H305" t="inlineStr">
@@ -17442,7 +17442,7 @@
       </c>
       <c r="G306" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H306" t="inlineStr">
@@ -17496,7 +17496,7 @@
       </c>
       <c r="G307" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H307" t="inlineStr">
@@ -17550,7 +17550,7 @@
       </c>
       <c r="G308" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H308" t="inlineStr">
@@ -17604,7 +17604,7 @@
       </c>
       <c r="G309" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H309" t="inlineStr">
@@ -17658,7 +17658,7 @@
       </c>
       <c r="G310" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H310" t="inlineStr">
@@ -17712,7 +17712,7 @@
       </c>
       <c r="G311" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SUBHASH CHAND</t>
         </is>
       </c>
       <c r="H311" t="inlineStr">
@@ -17766,7 +17766,7 @@
       </c>
       <c r="G312" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H312" t="inlineStr">
@@ -17820,7 +17820,7 @@
       </c>
       <c r="G313" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H313" t="inlineStr">
@@ -17874,7 +17874,7 @@
       </c>
       <c r="G314" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H314" t="inlineStr">
@@ -17928,7 +17928,7 @@
       </c>
       <c r="G315" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H315" t="inlineStr">
@@ -17982,7 +17982,7 @@
       </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H316" t="inlineStr">
@@ -18036,7 +18036,7 @@
       </c>
       <c r="G317" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H317" t="inlineStr">
@@ -18090,7 +18090,7 @@
       </c>
       <c r="G318" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H318" t="inlineStr">
@@ -18150,7 +18150,7 @@
       </c>
       <c r="G319" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H319" t="inlineStr">
@@ -18204,7 +18204,7 @@
       </c>
       <c r="G320" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H320" t="inlineStr">
@@ -18258,7 +18258,7 @@
       </c>
       <c r="G321" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H321" t="inlineStr">
@@ -18312,7 +18312,7 @@
       </c>
       <c r="G322" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H322" t="inlineStr">
@@ -18372,7 +18372,7 @@
       </c>
       <c r="G323" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H323" t="inlineStr">
@@ -18432,7 +18432,7 @@
       </c>
       <c r="G324" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H324" t="inlineStr">
@@ -18486,7 +18486,7 @@
       </c>
       <c r="G325" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H325" t="inlineStr">
@@ -18540,7 +18540,7 @@
       </c>
       <c r="G326" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SURESH</t>
         </is>
       </c>
       <c r="H326" t="inlineStr">
@@ -18594,7 +18594,7 @@
       </c>
       <c r="G327" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H327" t="inlineStr">
@@ -18648,7 +18648,7 @@
       </c>
       <c r="G328" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H328" t="inlineStr">
@@ -18702,7 +18702,7 @@
       </c>
       <c r="G329" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H329" t="inlineStr">
@@ -18762,7 +18762,7 @@
       </c>
       <c r="G330" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H330" t="inlineStr">
@@ -18822,7 +18822,7 @@
       </c>
       <c r="G331" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H331" t="inlineStr">
@@ -18876,7 +18876,7 @@
       </c>
       <c r="G332" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H332" t="inlineStr">
@@ -18930,7 +18930,7 @@
       </c>
       <c r="G333" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H333" t="inlineStr">
@@ -18984,7 +18984,7 @@
       </c>
       <c r="G334" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H334" t="inlineStr">
@@ -19044,7 +19044,7 @@
       </c>
       <c r="G335" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H335" t="inlineStr">
@@ -19098,7 +19098,7 @@
       </c>
       <c r="G336" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>RAJENDER KUMAR VERMA</t>
         </is>
       </c>
       <c r="H336" t="inlineStr">
@@ -19152,7 +19152,7 @@
       </c>
       <c r="G337" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H337" t="inlineStr">
@@ -19206,7 +19206,7 @@
       </c>
       <c r="G338" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H338" t="inlineStr">
@@ -19260,7 +19260,7 @@
       </c>
       <c r="G339" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H339" t="inlineStr">
@@ -19314,7 +19314,7 @@
       </c>
       <c r="G340" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H340" t="inlineStr">
@@ -19368,7 +19368,7 @@
       </c>
       <c r="G341" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H341" t="inlineStr">
@@ -19422,7 +19422,7 @@
       </c>
       <c r="G342" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H342" t="inlineStr">
@@ -19476,7 +19476,7 @@
       </c>
       <c r="G343" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H343" t="inlineStr">
@@ -19530,7 +19530,7 @@
       </c>
       <c r="G344" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H344" t="inlineStr">
@@ -19584,7 +19584,7 @@
       </c>
       <c r="G345" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H345" t="inlineStr">
@@ -19644,7 +19644,7 @@
       </c>
       <c r="G346" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>RAJENDER KUMAR VERMA</t>
         </is>
       </c>
       <c r="H346" t="inlineStr">
@@ -19698,7 +19698,7 @@
       </c>
       <c r="G347" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H347" t="inlineStr">
@@ -19758,7 +19758,7 @@
       </c>
       <c r="G348" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SURESH</t>
         </is>
       </c>
       <c r="H348" t="inlineStr">
@@ -19812,7 +19812,7 @@
       </c>
       <c r="G349" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H349" t="inlineStr">
@@ -19866,7 +19866,7 @@
       </c>
       <c r="G350" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H350" t="inlineStr">
@@ -19920,7 +19920,7 @@
       </c>
       <c r="G351" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H351" t="inlineStr">
@@ -19974,7 +19974,7 @@
       </c>
       <c r="G352" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>BEENESH</t>
         </is>
       </c>
       <c r="H352" t="inlineStr">
@@ -20034,7 +20034,7 @@
       </c>
       <c r="G353" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H353" t="inlineStr">
@@ -20094,7 +20094,7 @@
       </c>
       <c r="G354" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H354" t="inlineStr">
@@ -20148,7 +20148,7 @@
       </c>
       <c r="G355" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H355" t="inlineStr">
@@ -20208,7 +20208,7 @@
       </c>
       <c r="G356" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H356" t="inlineStr">
@@ -20262,7 +20262,7 @@
       </c>
       <c r="G357" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H357" t="inlineStr">
@@ -20322,7 +20322,7 @@
       </c>
       <c r="G358" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H358" t="inlineStr">
@@ -20382,7 +20382,7 @@
       </c>
       <c r="G359" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H359" t="inlineStr">
@@ -20436,7 +20436,7 @@
       </c>
       <c r="G360" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H360" t="inlineStr">
@@ -20496,7 +20496,7 @@
       </c>
       <c r="G361" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H361" t="inlineStr">
@@ -20550,7 +20550,7 @@
       </c>
       <c r="G362" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H362" t="inlineStr">
@@ -20604,7 +20604,7 @@
       </c>
       <c r="G363" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H363" t="inlineStr">
@@ -20664,7 +20664,7 @@
       </c>
       <c r="G364" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H364" t="inlineStr">
@@ -20718,7 +20718,7 @@
       </c>
       <c r="G365" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H365" t="inlineStr">
@@ -20772,7 +20772,7 @@
       </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H366" t="inlineStr">
@@ -20826,7 +20826,7 @@
       </c>
       <c r="G367" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>ANIL KUMAR PANDIT</t>
         </is>
       </c>
       <c r="H367" t="inlineStr">
@@ -20880,7 +20880,7 @@
       </c>
       <c r="G368" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H368" t="inlineStr">
@@ -20934,7 +20934,7 @@
       </c>
       <c r="G369" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H369" t="inlineStr">
@@ -20988,7 +20988,7 @@
       </c>
       <c r="G370" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>SHAKEEL</t>
         </is>
       </c>
       <c r="H370" t="inlineStr">
@@ -21042,7 +21042,7 @@
       </c>
       <c r="G371" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H371" t="inlineStr">
@@ -21102,7 +21102,7 @@
       </c>
       <c r="G372" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H372" t="inlineStr">
@@ -21156,7 +21156,7 @@
       </c>
       <c r="G373" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H373" t="inlineStr">
@@ -21216,7 +21216,7 @@
       </c>
       <c r="G374" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H374" t="inlineStr">
@@ -21270,7 +21270,7 @@
       </c>
       <c r="G375" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H375" t="inlineStr">
@@ -21324,7 +21324,7 @@
       </c>
       <c r="G376" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H376" t="inlineStr">
@@ -21378,7 +21378,7 @@
       </c>
       <c r="G377" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H377" t="inlineStr">
@@ -21432,7 +21432,7 @@
       </c>
       <c r="G378" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H378" t="inlineStr">
@@ -21492,7 +21492,7 @@
       </c>
       <c r="G379" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H379" t="inlineStr">
@@ -21552,7 +21552,7 @@
       </c>
       <c r="G380" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H380" t="inlineStr">
@@ -21606,7 +21606,7 @@
       </c>
       <c r="G381" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H381" t="inlineStr">
@@ -21660,7 +21660,7 @@
       </c>
       <c r="G382" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H382" t="inlineStr">
@@ -21714,7 +21714,7 @@
       </c>
       <c r="G383" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H383" t="inlineStr">
@@ -21768,7 +21768,7 @@
       </c>
       <c r="G384" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H384" t="inlineStr">
@@ -21828,7 +21828,7 @@
       </c>
       <c r="G385" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H385" t="inlineStr">
@@ -21882,7 +21882,7 @@
       </c>
       <c r="G386" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H386" t="inlineStr">
@@ -21936,7 +21936,7 @@
       </c>
       <c r="G387" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H387" t="inlineStr">
@@ -21990,7 +21990,7 @@
       </c>
       <c r="G388" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H388" t="inlineStr">
@@ -22044,7 +22044,7 @@
       </c>
       <c r="G389" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>PRAMOD-JAIPUR</t>
         </is>
       </c>
       <c r="H389" t="inlineStr">
@@ -22098,7 +22098,7 @@
       </c>
       <c r="G390" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H390" t="inlineStr">
@@ -22158,7 +22158,7 @@
       </c>
       <c r="G391" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H391" t="inlineStr">
@@ -22212,7 +22212,7 @@
       </c>
       <c r="G392" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H392" t="inlineStr">
@@ -22266,7 +22266,7 @@
       </c>
       <c r="G393" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H393" t="inlineStr">
@@ -22320,7 +22320,7 @@
       </c>
       <c r="G394" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H394" t="inlineStr">
@@ -22374,7 +22374,7 @@
       </c>
       <c r="G395" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H395" t="inlineStr">
@@ -22428,7 +22428,7 @@
       </c>
       <c r="G396" t="inlineStr">
         <is>
-          <t>--</t>
+          <t>NO FOS</t>
         </is>
       </c>
       <c r="H396" t="inlineStr">

</xml_diff>